<commit_message>
updates to test case definitions
</commit_message>
<xml_diff>
--- a/tests/test_cases.xlsx
+++ b/tests/test_cases.xlsx
@@ -343,10 +343,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -372,275 +372,240 @@
       <c r="A3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
+      <c r="B9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>44682</v>
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>44713</v>
+        <v>44682</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>45077</v>
+        <v>44713</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>120000</v>
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>45077</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>120000</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
+      <c r="B18" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2"/>
-      <c r="B20" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="3" t="n">
-        <v>44713</v>
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23" s="3" t="n">
-        <v>45077</v>
+        <v>44713</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
       <c r="B24" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>45077</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2"/>
+      <c r="B26" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="1" t="n">
-        <v>120000</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="C26" s="1" t="n">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="5" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2" t="s">
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I29" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L28" s="4" t="s">
+      <c r="L29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M28" s="4" t="s">
+      <c r="M29" s="4" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>0</v>
@@ -678,7 +643,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>0</v>
@@ -716,7 +681,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>0</v>
@@ -754,19 +719,19 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" s="0" t="n">
-        <v>120000</v>
-      </c>
-      <c r="F33" s="0" t="n">
-        <v>120000</v>
+      <c r="D33" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="6" t="n">
+        <v>0</v>
       </c>
       <c r="G33" s="6" t="n">
         <v>0</v>
@@ -792,31 +757,28 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" s="1" t="n">
-        <f aca="false">120000/12</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1" t="n">
-        <f aca="false">120000/12</f>
-        <v>10000</v>
-      </c>
-      <c r="E34" s="1" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>120000</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>120000</v>
       </c>
-      <c r="G34" s="0" t="n">
-        <v>120000</v>
-      </c>
-      <c r="H34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" s="0" t="n">
-        <f aca="false">120000/12</f>
-        <v>10000</v>
+      <c r="G34" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>0</v>
@@ -828,13 +790,12 @@
         <v>0</v>
       </c>
       <c r="M34" s="0" t="n">
-        <f aca="false">120000/12</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C35" s="1" t="n">
         <f aca="false">120000/12</f>
@@ -854,11 +815,11 @@
         <v>120000</v>
       </c>
       <c r="H35" s="0" t="n">
-        <f aca="false">120000/12</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="I35" s="0" t="n">
-        <v>0</v>
+        <f aca="false">120000/12</f>
+        <v>10000</v>
       </c>
       <c r="J35" s="0" t="n">
         <v>0</v>
@@ -876,7 +837,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C36" s="1" t="n">
         <f aca="false">120000/12</f>
@@ -918,7 +879,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" s="1" t="n">
         <f aca="false">120000/12</f>
@@ -960,7 +921,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" s="1" t="n">
         <f aca="false">120000/12</f>
@@ -1002,7 +963,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" s="1" t="n">
         <f aca="false">120000/12</f>
@@ -1044,7 +1005,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" s="1" t="n">
         <f aca="false">120000/12</f>
@@ -1086,7 +1047,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C41" s="1" t="n">
         <f aca="false">120000/12</f>
@@ -1128,7 +1089,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C42" s="1" t="n">
         <f aca="false">120000/12</f>
@@ -1170,7 +1131,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" s="1" t="n">
         <f aca="false">120000/12</f>
@@ -1212,7 +1173,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" s="1" t="n">
         <f aca="false">120000/12</f>
@@ -1254,7 +1215,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C45" s="1" t="n">
         <f aca="false">120000/12</f>
@@ -1296,24 +1257,27 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>0</v>
+        <f aca="false">120000/12</f>
+        <v>10000</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>0</v>
+        <f aca="false">120000/12</f>
+        <v>10000</v>
       </c>
       <c r="E46" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F46" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" s="1" t="n">
-        <v>0</v>
+      <c r="F46" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>120000</v>
       </c>
       <c r="H46" s="0" t="n">
+        <f aca="false">120000/12</f>
         <v>10000</v>
       </c>
       <c r="I46" s="0" t="n">
@@ -1323,18 +1287,19 @@
         <v>0</v>
       </c>
       <c r="K46" s="0" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="L46" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M46" s="0" t="n">
-        <v>0</v>
+        <f aca="false">120000/12</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>0</v>
@@ -1351,8 +1316,8 @@
       <c r="G47" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H47" s="1" t="n">
-        <v>0</v>
+      <c r="H47" s="0" t="n">
+        <v>10000</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>0</v>
@@ -1361,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="K47" s="0" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="L47" s="0" t="n">
         <v>0</v>
@@ -1372,7 +1337,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>0</v>
@@ -1410,7 +1375,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>0</v>
@@ -1448,7 +1413,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>0</v>
@@ -1486,7 +1451,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>0</v>
@@ -1524,45 +1489,83 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H52" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M52" s="0" t="n">
+      <c r="C53" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" s="0" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="H28:M28"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2857,7 +2860,7 @@
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M47" activeCellId="0" sqref="M47"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
implemented contract lengths != 12
</commit_message>
<xml_diff>
--- a/tests/test_cases.xlsx
+++ b/tests/test_cases.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="case1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="case2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="case3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="case4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="66">
   <si>
     <t xml:space="preserve">Case 1</t>
   </si>
@@ -217,6 +218,9 @@
   </si>
   <si>
     <t xml:space="preserve">Single 12-Month Contract, $120k, renewed at end with half ARR $60k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single 6-Month Contract, $60k total value</t>
   </si>
 </sst>
 </file>
@@ -232,6 +236,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -253,6 +258,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -318,7 +324,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -346,15 +352,15 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="G40:G52 C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="13.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1585,15 +1591,15 @@
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H58" activeCellId="0" sqref="H58"/>
+      <selection pane="topLeft" activeCell="H58" activeCellId="1" sqref="G40:G52 H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="13.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,16 +2865,16 @@
   </sheetPr>
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E34" activeCellId="1" sqref="G40:G52 E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="13.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4111,6 +4117,1228 @@
       </c>
       <c r="M52" s="0" t="n">
         <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H27:M27"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M52"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40:G52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="13.71"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2"/>
+      <c r="B11" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
+      <c r="B12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2"/>
+      <c r="B13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>44682</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+      <c r="B14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>44713</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2"/>
+      <c r="B15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>44895</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2"/>
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>60000</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+      <c r="B17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2"/>
+      <c r="B20" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
+      <c r="B21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
+      <c r="B22" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>44713</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="B23" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>44895</v>
+      </c>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2"/>
+      <c r="B24" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2"/>
+      <c r="B25" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>60000</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="G33" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <f aca="false">120000/12</f>
+        <v>10000</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M50" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>